<commit_message>
Ajustements guide - neutre
- Ajout mécanos liste
- Ajustement matériel neutre
</commit_message>
<xml_diff>
--- a/excel/ardoise_info_neutre.xlsx
+++ b/excel/ardoise_info_neutre.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10514"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10611"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/brunogauthier/Documents/guide2023/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D02C7C95-FF8B-3D4B-B4B2-DF34DF0DBF21}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1EF2B0C6-5104-2349-93FE-A3F2422128C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="20500" xr2:uid="{FD29B0F2-1663-8540-80A1-3F866C889E60}"/>
+    <workbookView xWindow="69560" yWindow="3980" windowWidth="33600" windowHeight="20500" activeTab="2" xr2:uid="{FD29B0F2-1663-8540-80A1-3F866C889E60}"/>
   </bookViews>
   <sheets>
     <sheet name="COORD" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
     <sheet name="COORD_DEP" sheetId="5" r:id="rId3"/>
     <sheet name="HORAIRE_DEP" sheetId="6" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="50">
   <si>
     <t>Bruno Gauthier</t>
   </si>
@@ -153,6 +153,42 @@
   </si>
   <si>
     <t>\(819) 443-2700</t>
+  </si>
+  <si>
+    <t>Hubert Lamothe</t>
+  </si>
+  <si>
+    <t>\(819) 444-1380</t>
+  </si>
+  <si>
+    <t>Louis Coteau</t>
+  </si>
+  <si>
+    <t>Conducteur Marc Dufour</t>
+  </si>
+  <si>
+    <t>Conducteur moto</t>
+  </si>
+  <si>
+    <t>Conducteur auto Centrifuge</t>
+  </si>
+  <si>
+    <t>Back-up</t>
+  </si>
+  <si>
+    <t>Non contacté 2023</t>
+  </si>
+  <si>
+    <t>Félix-Antoine Malo</t>
+  </si>
+  <si>
+    <t>felixantoine.malo@gmail.com</t>
+  </si>
+  <si>
+    <t>(514) 994-8760</t>
+  </si>
+  <si>
+    <t>Conducteur Tour</t>
   </si>
 </sst>
 </file>
@@ -212,7 +248,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="20">
+  <borders count="19">
     <border>
       <left/>
       <right/>
@@ -311,17 +347,6 @@
     </border>
     <border>
       <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
         <color indexed="64"/>
       </left>
       <right/>
@@ -430,7 +455,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -468,14 +493,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -800,7 +824,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{72262817-9D66-6D48-97C4-5126E8F8BB18}">
   <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A34" sqref="A34"/>
     </sheetView>
   </sheetViews>
@@ -996,10 +1020,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{53EDA790-0658-EF4E-9D2F-BE0EFC66A120}">
-  <dimension ref="A1:D9"/>
+  <dimension ref="A1:D16"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="A32" sqref="A32"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="A30" sqref="A30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1033,17 +1057,35 @@
         <v>34</v>
       </c>
       <c r="D2" t="s">
-        <v>25</v>
+        <v>42</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>41</v>
+      </c>
+      <c r="B3" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D3" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>13</v>
+        <v>46</v>
+      </c>
+      <c r="B4" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="C4" t="s">
+        <v>48</v>
+      </c>
+      <c r="D4" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
@@ -1056,6 +1098,9 @@
       <c r="C7" t="s">
         <v>35</v>
       </c>
+      <c r="D7" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
@@ -1064,6 +1109,9 @@
       <c r="C8" t="s">
         <v>36</v>
       </c>
+      <c r="D8" t="s">
+        <v>45</v>
+      </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
@@ -1072,10 +1120,43 @@
       <c r="C9" t="s">
         <v>37</v>
       </c>
+      <c r="D9" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>38</v>
+      </c>
+      <c r="C11" t="s">
+        <v>39</v>
+      </c>
+      <c r="D11" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>40</v>
+      </c>
+      <c r="D12" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>13</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B7" r:id="rId1" xr:uid="{E9D7E016-9946-E84B-BD28-6C130476923D}"/>
+    <hyperlink ref="B4" r:id="rId2" xr:uid="{EA584547-6977-7341-AED4-4AFF87F29DD3}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
@@ -1087,7 +1168,7 @@
   <dimension ref="A1:H8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="21" x14ac:dyDescent="0.25"/>
@@ -1101,80 +1182,81 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="20" t="s">
+      <c r="A1" s="19" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="21" t="s">
+      <c r="B1" s="20" t="s">
         <v>19</v>
       </c>
-      <c r="C1" s="22" t="s">
+      <c r="C1" s="21" t="s">
         <v>26</v>
       </c>
-      <c r="D1" s="23" t="s">
+      <c r="D1" s="22" t="s">
         <v>20</v>
       </c>
-      <c r="E1" s="23" t="s">
+      <c r="E1" s="22" t="s">
         <v>27</v>
       </c>
-      <c r="F1" s="21" t="s">
+      <c r="F1" s="20" t="s">
         <v>21</v>
       </c>
-      <c r="G1" s="22" t="s">
+      <c r="G1" s="21" t="s">
         <v>28</v>
       </c>
-      <c r="H1" s="24" t="s">
+      <c r="H1" s="23" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="25">
+    <row r="2" spans="1:8" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="24">
         <v>1</v>
       </c>
-      <c r="B2" s="26" t="s">
+      <c r="B2" s="25" t="s">
+        <v>38</v>
+      </c>
+      <c r="C2" s="26" t="s">
+        <v>41</v>
+      </c>
+      <c r="D2" s="27" t="s">
+        <v>40</v>
+      </c>
+      <c r="E2" s="26" t="s">
         <v>22</v>
       </c>
-      <c r="C2" s="27" t="s">
+      <c r="F2" s="27" t="s">
         <v>4</v>
       </c>
-      <c r="D2" s="28" t="s">
-        <v>4</v>
-      </c>
-      <c r="E2" s="27" t="s">
-        <v>4</v>
-      </c>
-      <c r="F2" s="28" t="s">
-        <v>4</v>
-      </c>
-      <c r="G2" s="29" t="s">
-        <v>4</v>
-      </c>
-      <c r="H2" s="29"/>
+      <c r="G2" s="28" t="s">
+        <v>46</v>
+      </c>
+      <c r="H2" s="28"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="13">
         <v>2</v>
       </c>
-      <c r="B3" s="11" t="s">
+      <c r="B3" s="25" t="s">
+        <v>38</v>
+      </c>
+      <c r="C3" s="12" t="str">
+        <f>C2</f>
+        <v>Conducteur Marc Dufour</v>
+      </c>
+      <c r="D3" s="27" t="s">
+        <v>40</v>
+      </c>
+      <c r="E3" s="12" t="s">
         <v>22</v>
-      </c>
-      <c r="C3" s="12" t="s">
-        <v>4</v>
-      </c>
-      <c r="D3" t="s">
-        <v>4</v>
-      </c>
-      <c r="E3" s="12" t="s">
-        <v>4</v>
       </c>
       <c r="F3" t="s">
         <v>4</v>
       </c>
       <c r="G3" s="14" t="s">
-        <v>4</v>
+        <v>46</v>
       </c>
       <c r="H3" s="14"/>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" ht="22" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="13">
         <v>3</v>
       </c>
@@ -1182,13 +1264,13 @@
         <v>22</v>
       </c>
       <c r="C4" s="12" t="s">
-        <v>4</v>
+        <v>13</v>
       </c>
       <c r="D4" t="s">
-        <v>4</v>
+        <v>41</v>
       </c>
       <c r="E4" s="12" t="s">
-        <v>4</v>
+        <v>13</v>
       </c>
       <c r="F4" t="s">
         <v>13</v>
@@ -1200,75 +1282,77 @@
         <v>23</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" ht="22" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="13">
         <v>4</v>
       </c>
-      <c r="B5" s="11" t="s">
+      <c r="B5" s="25" t="s">
+        <v>38</v>
+      </c>
+      <c r="C5" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="D5" s="27" t="s">
+        <v>40</v>
+      </c>
+      <c r="E5" s="12" t="s">
         <v>22</v>
-      </c>
-      <c r="C5" s="12" t="s">
-        <v>4</v>
-      </c>
-      <c r="D5" t="s">
-        <v>4</v>
-      </c>
-      <c r="E5" s="12" t="s">
-        <v>4</v>
       </c>
       <c r="F5" t="s">
         <v>4</v>
       </c>
       <c r="G5" s="14" t="s">
-        <v>4</v>
+        <v>46</v>
       </c>
       <c r="H5" s="14"/>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" ht="22" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="13">
         <v>5</v>
       </c>
-      <c r="B6" s="11" t="s">
+      <c r="B6" s="25" t="s">
+        <v>38</v>
+      </c>
+      <c r="C6" s="12" t="str">
+        <f t="shared" ref="C6:C8" si="0">C5</f>
+        <v>Conducteur Marc Dufour</v>
+      </c>
+      <c r="D6" s="27" t="s">
+        <v>40</v>
+      </c>
+      <c r="E6" s="12" t="s">
         <v>22</v>
-      </c>
-      <c r="C6" s="12" t="s">
-        <v>4</v>
-      </c>
-      <c r="D6" t="s">
-        <v>4</v>
-      </c>
-      <c r="E6" s="12" t="s">
-        <v>4</v>
       </c>
       <c r="F6" t="s">
         <v>4</v>
       </c>
       <c r="G6" s="14" t="s">
-        <v>4</v>
+        <v>46</v>
       </c>
       <c r="H6" s="14"/>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" ht="22" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="13">
         <v>6</v>
       </c>
-      <c r="B7" s="11" t="s">
+      <c r="B7" s="25" t="s">
+        <v>38</v>
+      </c>
+      <c r="C7" s="12" t="str">
+        <f t="shared" si="0"/>
+        <v>Conducteur Marc Dufour</v>
+      </c>
+      <c r="D7" s="27" t="s">
+        <v>40</v>
+      </c>
+      <c r="E7" s="12" t="s">
         <v>22</v>
-      </c>
-      <c r="C7" s="12" t="s">
-        <v>4</v>
-      </c>
-      <c r="D7" t="s">
-        <v>4</v>
-      </c>
-      <c r="E7" s="12" t="s">
-        <v>4</v>
       </c>
       <c r="F7" t="s">
         <v>4</v>
       </c>
       <c r="G7" s="14" t="s">
-        <v>4</v>
+        <v>46</v>
       </c>
       <c r="H7" s="14"/>
     </row>
@@ -1276,25 +1360,26 @@
       <c r="A8" s="15">
         <v>7</v>
       </c>
-      <c r="B8" s="16" t="s">
+      <c r="B8" s="25" t="s">
+        <v>38</v>
+      </c>
+      <c r="C8" s="12" t="str">
+        <f t="shared" si="0"/>
+        <v>Conducteur Marc Dufour</v>
+      </c>
+      <c r="D8" s="27" t="s">
+        <v>40</v>
+      </c>
+      <c r="E8" s="16" t="s">
         <v>22</v>
       </c>
-      <c r="C8" s="17" t="s">
+      <c r="F8" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="D8" s="18" t="s">
-        <v>4</v>
-      </c>
-      <c r="E8" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="F8" s="18" t="s">
-        <v>4</v>
-      </c>
-      <c r="G8" s="19" t="s">
-        <v>4</v>
-      </c>
-      <c r="H8" s="19"/>
+      <c r="G8" s="18" t="s">
+        <v>46</v>
+      </c>
+      <c r="H8" s="18"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
correction chauffeur dep neutre
</commit_message>
<xml_diff>
--- a/excel/ardoise_info_neutre.xlsx
+++ b/excel/ardoise_info_neutre.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/brunogauthier/Documents/guide2023/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43E417C3-3518-7E4F-AA36-195C506021D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D376A02-39FB-F746-9F3D-FAEE3B301B30}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="26600" yWindow="3160" windowWidth="33600" windowHeight="20500" activeTab="3" xr2:uid="{FD29B0F2-1663-8540-80A1-3F866C889E60}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="20500" activeTab="3" xr2:uid="{FD29B0F2-1663-8540-80A1-3F866C889E60}"/>
   </bookViews>
   <sheets>
     <sheet name="COORD" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="56">
   <si>
     <t>Bruno Gauthier</t>
   </si>
@@ -192,13 +192,28 @@
   </si>
   <si>
     <t>Guillaume à confirmer</t>
+  </si>
+  <si>
+    <t>Daniel Asselin</t>
+  </si>
+  <si>
+    <t>Serge Bernier</t>
+  </si>
+  <si>
+    <t>dasselin@ulsat.qc.ca</t>
+  </si>
+  <si>
+    <t>\(819) 856-4608</t>
+  </si>
+  <si>
+    <t>Jeannot Dionne</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -242,6 +257,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -458,7 +480,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -510,6 +532,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Lien hypertexte" xfId="1" builtinId="8"/>
@@ -1026,7 +1049,7 @@
   <dimension ref="A1:D15"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="A20" sqref="A20"/>
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1088,6 +1111,28 @@
         <v>45</v>
       </c>
     </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>51</v>
+      </c>
+      <c r="B5" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="D5" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>52</v>
+      </c>
+      <c r="C6" t="s">
+        <v>54</v>
+      </c>
+      <c r="D6" t="s">
+        <v>45</v>
+      </c>
+    </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>29</v>
@@ -1144,6 +1189,14 @@
       </c>
       <c r="D11" t="s">
         <v>25</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>55</v>
+      </c>
+      <c r="D12" s="29" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
@@ -1160,6 +1213,7 @@
   <hyperlinks>
     <hyperlink ref="B7" r:id="rId1" xr:uid="{E9D7E016-9946-E84B-BD28-6C130476923D}"/>
     <hyperlink ref="B4" r:id="rId2" xr:uid="{A6E45AC4-6E75-A14D-BE23-221703F69315}"/>
+    <hyperlink ref="B5" r:id="rId3" xr:uid="{8AF601C5-A5CE-E246-8B0C-3221C9BFAEF2}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
@@ -1171,7 +1225,7 @@
   <dimension ref="A1:H8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="21" x14ac:dyDescent="0.25"/>
@@ -1230,7 +1284,7 @@
         <v>29</v>
       </c>
       <c r="G2" s="28" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="H2" s="28"/>
     </row>
@@ -1255,7 +1309,7 @@
         <v>49</v>
       </c>
       <c r="G3" s="14" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="H3" s="14"/>
     </row>
@@ -1305,7 +1359,7 @@
         <v>29</v>
       </c>
       <c r="G5" s="14" t="s">
-        <v>47</v>
+        <v>55</v>
       </c>
       <c r="H5" s="14"/>
     </row>
@@ -1330,7 +1384,7 @@
         <v>49</v>
       </c>
       <c r="G6" s="14" t="s">
-        <v>47</v>
+        <v>52</v>
       </c>
       <c r="H6" s="14"/>
     </row>
@@ -1355,7 +1409,7 @@
         <v>29</v>
       </c>
       <c r="G7" s="14" t="s">
-        <v>47</v>
+        <v>52</v>
       </c>
       <c r="H7" s="14"/>
     </row>
@@ -1380,7 +1434,7 @@
         <v>29</v>
       </c>
       <c r="G8" s="18" t="s">
-        <v>47</v>
+        <v>52</v>
       </c>
       <c r="H8" s="18" t="s">
         <v>50</v>

</xml_diff>

<commit_message>
correction liste dep neutre
</commit_message>
<xml_diff>
--- a/excel/ardoise_info_neutre.xlsx
+++ b/excel/ardoise_info_neutre.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10611"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/brunogauthier/Documents/guide2023/excel/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pierrick.naud\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D376A02-39FB-F746-9F3D-FAEE3B301B30}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{19C15543-76B2-4EB0-8BF5-EF3A438D6336}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="20500" activeTab="3" xr2:uid="{FD29B0F2-1663-8540-80A1-3F866C889E60}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" activeTab="3" xr2:uid="{FD29B0F2-1663-8540-80A1-3F866C889E60}"/>
   </bookViews>
   <sheets>
     <sheet name="COORD" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
     <sheet name="COORD_DEP" sheetId="5" r:id="rId3"/>
     <sheet name="HORAIRE_DEP" sheetId="6" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="191029" concurrentCalc="0"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="56">
   <si>
     <t>Bruno Gauthier</t>
   </si>
@@ -191,9 +191,6 @@
     <t>Jérôme Sayeur</t>
   </si>
   <si>
-    <t>Guillaume à confirmer</t>
-  </si>
-  <si>
     <t>Daniel Asselin</t>
   </si>
   <si>
@@ -207,6 +204,9 @@
   </si>
   <si>
     <t>Jeannot Dionne</t>
+  </si>
+  <si>
+    <t>Maude Ébacher</t>
   </si>
 </sst>
 </file>
@@ -854,14 +854,14 @@
       <selection activeCell="A34" sqref="A34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.796875" defaultRowHeight="15" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="2" width="61.1640625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="64.33203125" style="1" customWidth="1"/>
-    <col min="4" max="16384" width="10.83203125" style="1"/>
+    <col min="1" max="2" width="61.19921875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="64.296875" style="1" customWidth="1"/>
+    <col min="4" max="16384" width="10.796875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" s="3" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>14</v>
       </c>
@@ -872,7 +872,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
@@ -883,7 +883,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -894,7 +894,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>0</v>
       </c>
@@ -924,15 +924,15 @@
       <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="21" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="21" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="14.1640625" style="8" customWidth="1"/>
-    <col min="2" max="2" width="23.6640625" customWidth="1"/>
-    <col min="3" max="3" width="24.33203125" customWidth="1"/>
-    <col min="5" max="8" width="30.6640625" customWidth="1"/>
+    <col min="1" max="1" width="14.19921875" style="8" customWidth="1"/>
+    <col min="2" max="2" width="23.69921875" customWidth="1"/>
+    <col min="3" max="3" width="24.296875" customWidth="1"/>
+    <col min="5" max="8" width="30.69921875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" s="6" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A1" s="7" t="s">
         <v>11</v>
       </c>
@@ -946,7 +946,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A2" s="8">
         <v>1</v>
       </c>
@@ -957,7 +957,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A3" s="8">
         <v>2</v>
       </c>
@@ -968,7 +968,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A4" s="8">
         <v>3</v>
       </c>
@@ -982,7 +982,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A5" s="8">
         <v>4</v>
       </c>
@@ -993,7 +993,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A6" s="8">
         <v>5</v>
       </c>
@@ -1004,7 +1004,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A7" s="8">
         <v>6</v>
       </c>
@@ -1015,7 +1015,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A8" s="8">
         <v>7</v>
       </c>
@@ -1049,16 +1049,16 @@
   <dimension ref="A1:D15"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="3" width="49.5" customWidth="1"/>
-    <col min="4" max="4" width="34.1640625" customWidth="1"/>
+    <col min="4" max="4" width="34.19921875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>14</v>
       </c>
@@ -1072,7 +1072,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>22</v>
       </c>
@@ -1086,7 +1086,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>41</v>
       </c>
@@ -1100,7 +1100,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>47</v>
       </c>
@@ -1111,29 +1111,29 @@
         <v>45</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B5" s="10" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D5" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C6" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D6" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>29</v>
       </c>
@@ -1147,7 +1147,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>31</v>
       </c>
@@ -1158,7 +1158,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>32</v>
       </c>
@@ -1169,7 +1169,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>38</v>
       </c>
@@ -1180,7 +1180,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>40</v>
       </c>
@@ -1191,20 +1191,28 @@
         <v>25</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D12" s="29" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>55</v>
+      </c>
+      <c r="D13" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>13</v>
       </c>
@@ -1225,20 +1233,20 @@
   <dimension ref="A1:H8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="21" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="21" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="14.1640625" style="8" customWidth="1"/>
-    <col min="2" max="4" width="17.6640625" customWidth="1"/>
-    <col min="5" max="5" width="21.1640625" customWidth="1"/>
-    <col min="6" max="6" width="17.6640625" customWidth="1"/>
-    <col min="7" max="7" width="21.1640625" customWidth="1"/>
-    <col min="8" max="8" width="48.1640625" customWidth="1"/>
+    <col min="1" max="1" width="14.19921875" style="8" customWidth="1"/>
+    <col min="2" max="4" width="17.69921875" customWidth="1"/>
+    <col min="5" max="5" width="21.19921875" customWidth="1"/>
+    <col min="6" max="6" width="17.69921875" customWidth="1"/>
+    <col min="7" max="7" width="21.19921875" customWidth="1"/>
+    <col min="8" max="8" width="48.19921875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A1" s="19" t="s">
         <v>11</v>
       </c>
@@ -1264,7 +1272,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A2" s="24">
         <v>1</v>
       </c>
@@ -1284,11 +1292,11 @@
         <v>29</v>
       </c>
       <c r="G2" s="28" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="H2" s="28"/>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A3" s="13">
         <v>2</v>
       </c>
@@ -1309,11 +1317,11 @@
         <v>49</v>
       </c>
       <c r="G3" s="14" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="H3" s="14"/>
     </row>
-    <row r="4" spans="1:8" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A4" s="13">
         <v>3</v>
       </c>
@@ -1339,7 +1347,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A5" s="13">
         <v>4</v>
       </c>
@@ -1359,11 +1367,11 @@
         <v>29</v>
       </c>
       <c r="G5" s="14" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="H5" s="14"/>
     </row>
-    <row r="6" spans="1:8" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A6" s="13">
         <v>5</v>
       </c>
@@ -1384,16 +1392,16 @@
         <v>49</v>
       </c>
       <c r="G6" s="14" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="H6" s="14"/>
     </row>
-    <row r="7" spans="1:8" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A7" s="13">
         <v>6</v>
       </c>
       <c r="B7" s="25" t="s">
-        <v>38</v>
+        <v>55</v>
       </c>
       <c r="C7" s="12" t="str">
         <f t="shared" si="0"/>
@@ -1409,11 +1417,11 @@
         <v>29</v>
       </c>
       <c r="G7" s="14" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="H7" s="14"/>
     </row>
-    <row r="8" spans="1:8" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A8" s="15">
         <v>7</v>
       </c>
@@ -1431,27 +1439,31 @@
         <v>22</v>
       </c>
       <c r="F8" s="17" t="s">
-        <v>29</v>
+        <v>55</v>
       </c>
       <c r="G8" s="18" t="s">
-        <v>52</v>
-      </c>
-      <c r="H8" s="18" t="s">
-        <v>50</v>
-      </c>
+        <v>51</v>
+      </c>
+      <c r="H8" s="18"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{2FF631A4-0570-384A-95CA-9C4F7FFE55C4}">
           <x14:formula1>
             <xm:f>COORD_DEP!$A$2:$A$18</xm:f>
           </x14:formula1>
           <xm:sqref>B2:E8 G2:G8</xm:sqref>
         </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{58D354B3-A020-544F-A500-46EE14A63744}">
+          <x14:formula1>
+            <xm:f>COORD_DEP!$A$2:$A$15</xm:f>
+          </x14:formula1>
+          <xm:sqref>F2:F8</xm:sqref>
+        </x14:dataValidation>
       </x14:dataValidations>
     </ext>
   </extLst>

</xml_diff>